<commit_message>
added theplayer image to the screen
</commit_message>
<xml_diff>
--- a/TCT-database.xlsx
+++ b/TCT-database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waltersylvester/sei-cranberry-gobblers/project-1-the-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCD39407-2A61-A64E-934F-F8FC7A2CE69D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD14BCA2-987E-7941-A036-A6C481149DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{94078475-5FDC-3F47-8680-DE6E559C9F43}"/>
+    <workbookView xWindow="6080" yWindow="1560" windowWidth="24740" windowHeight="17440" xr2:uid="{94078475-5FDC-3F47-8680-DE6E559C9F43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Top</t>
   </si>
@@ -58,6 +58,45 @@
   </si>
   <si>
     <t>Career MLB Leaders through 2019</t>
+  </si>
+  <si>
+    <t>Clue 1</t>
+  </si>
+  <si>
+    <t>Clue 2</t>
+  </si>
+  <si>
+    <t>Clue 3</t>
+  </si>
+  <si>
+    <t>Minimum of 3000 PA career leaderboards for rate statistics.</t>
+  </si>
+  <si>
+    <t>12 Batting Titles</t>
+  </si>
+  <si>
+    <t>1 Triple Crown and 1 MVP win</t>
+  </si>
+  <si>
+    <t>Nicknamed the Georgia Peach</t>
+  </si>
+  <si>
+    <t>7 Batting Titles</t>
+  </si>
+  <si>
+    <t>2 Triple Crown and 7 MVP wins</t>
+  </si>
+  <si>
+    <t>Nicknamed Rajah</t>
+  </si>
+  <si>
+    <t>13 year career</t>
+  </si>
+  <si>
+    <t>Played for PHA, CLE, and CWS</t>
+  </si>
+  <si>
+    <t>3 time AL Triples leader</t>
   </si>
 </sst>
 </file>
@@ -111,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,6 +163,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,89 +478,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B0D4E5-8810-294C-AC52-50FE39A2C234}">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5">
-        <v>0.36620000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <f>A5+1</f>
+      <c r="C6" s="5">
+        <f>4189/11439</f>
+        <v>0.36620333945274935</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <f>A6+1</f>
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5">
-        <v>0.35849999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <f t="shared" ref="A7:A9" si="0">A6+1</f>
+      <c r="C7" s="5">
+        <f>2930/8173</f>
+        <v>0.35849749174109874</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <f t="shared" ref="A8:A10" si="0">A7+1</f>
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C8" s="5">
         <v>0.35580000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="5">
         <v>0.3493</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C10" s="5">
         <v>0.3458</v>
       </c>
     </row>

</xml_diff>

<commit_message>
increased AVG database to 5 players
</commit_message>
<xml_diff>
--- a/TCT-database.xlsx
+++ b/TCT-database.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waltersylvester/sei-cranberry-gobblers/project-1-the-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD14BCA2-987E-7941-A036-A6C481149DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDFA5C8-572E-4043-9591-910418CDF30C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6080" yWindow="1560" windowWidth="24740" windowHeight="17440" xr2:uid="{94078475-5FDC-3F47-8680-DE6E559C9F43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Top</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>3 time AL Triples leader</t>
+  </si>
+  <si>
+    <t>2 Batting Titles</t>
+  </si>
+  <si>
+    <t>11 year career</t>
+  </si>
+  <si>
+    <t>Born on March 4, 1897</t>
+  </si>
+  <si>
+    <t>16 year career</t>
+  </si>
+  <si>
+    <t>Played for PHI, WSH, and CLE</t>
   </si>
 </sst>
 </file>
@@ -104,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.0000_);[Red]\(#,##0.0000\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000_);[Red]\(#,##0.0000\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -162,7 +177,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -481,7 +496,7 @@
   <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,6 +612,15 @@
       <c r="C9" s="5">
         <v>0.3493</v>
       </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -609,6 +633,15 @@
       <c r="C10" s="5">
         <v>0.3458</v>
       </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created an array of images in the game object
</commit_message>
<xml_diff>
--- a/TCT-database.xlsx
+++ b/TCT-database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waltersylvester/sei-cranberry-gobblers/project-1-the-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDFA5C8-572E-4043-9591-910418CDF30C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2B163B-5D2B-E941-8D18-38CCD3CD50CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6080" yWindow="1560" windowWidth="24740" windowHeight="17440" xr2:uid="{94078475-5FDC-3F47-8680-DE6E559C9F43}"/>
   </bookViews>
@@ -496,7 +496,7 @@
   <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added HR and RBI data
</commit_message>
<xml_diff>
--- a/TCT-database.xlsx
+++ b/TCT-database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waltersylvester/sei-cranberry-gobblers/project-1-the-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2B163B-5D2B-E941-8D18-38CCD3CD50CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98335C80-2EDB-6E43-AF76-B7996E503B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6080" yWindow="1560" windowWidth="24740" windowHeight="17440" xr2:uid="{94078475-5FDC-3F47-8680-DE6E559C9F43}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>Top</t>
   </si>
@@ -78,9 +78,6 @@
     <t>1 Triple Crown and 1 MVP win</t>
   </si>
   <si>
-    <t>Nicknamed the Georgia Peach</t>
-  </si>
-  <si>
     <t>7 Batting Titles</t>
   </si>
   <si>
@@ -112,6 +109,102 @@
   </si>
   <si>
     <t>Played for PHI, WSH, and CLE</t>
+  </si>
+  <si>
+    <t>RBI</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Barry Bonds</t>
+  </si>
+  <si>
+    <t>Hank Aaron</t>
+  </si>
+  <si>
+    <t>Babe Ruth</t>
+  </si>
+  <si>
+    <t>Alex Rodriguez</t>
+  </si>
+  <si>
+    <t>Willie Mays</t>
+  </si>
+  <si>
+    <t>Albert Pujols</t>
+  </si>
+  <si>
+    <t>&lt;--through 2019</t>
+  </si>
+  <si>
+    <t>All-time BB leader</t>
+  </si>
+  <si>
+    <t>7 NL MVP wins and 12 Silver Slugger Awards</t>
+  </si>
+  <si>
+    <t>14-time All-Star and 8 Gold Glove awards</t>
+  </si>
+  <si>
+    <t>All-time RBI and TB leader</t>
+  </si>
+  <si>
+    <t>Last Negro league player on an MLB roster</t>
+  </si>
+  <si>
+    <t>21-time All-Star, held HR record for 33 years</t>
+  </si>
+  <si>
+    <t>All-time SLG leader</t>
+  </si>
+  <si>
+    <t>7-time World Series champion</t>
+  </si>
+  <si>
+    <t>1-time AL batting champ and 1-time AL ERA champion</t>
+  </si>
+  <si>
+    <t>14-time All-Star and 10 Silver Slugger awards</t>
+  </si>
+  <si>
+    <t>3 AL MVP wins</t>
+  </si>
+  <si>
+    <t>1st pick of 1993 draft</t>
+  </si>
+  <si>
+    <t>ROY in 1951, 24-time All-Star</t>
+  </si>
+  <si>
+    <t>2-time NL MVP and 12 Gold Glove awards</t>
+  </si>
+  <si>
+    <t>Nicknamed The Say Hey Kid</t>
+  </si>
+  <si>
+    <t>Nicknamed The Georgia Peach</t>
+  </si>
+  <si>
+    <t>Cap Anson</t>
+  </si>
+  <si>
+    <t>played for 27 seasons</t>
+  </si>
+  <si>
+    <t>4-time batting champion</t>
+  </si>
+  <si>
+    <t>possibly the first player with 3,000 hits</t>
+  </si>
+  <si>
+    <t>Career GDP leader</t>
+  </si>
+  <si>
+    <t>13th round pick in 1999</t>
+  </si>
+  <si>
+    <t>3-time MVP, 6-time Silver Slugger</t>
   </si>
 </sst>
 </file>
@@ -145,12 +238,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,8 +276,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,17 +594,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B0D4E5-8810-294C-AC52-50FE39A2C234}">
-  <dimension ref="A2:F10"/>
+  <dimension ref="A2:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -513,7 +614,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -521,10 +622,10 @@
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -544,7 +645,7 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="7">
         <f>4189/11439</f>
         <v>0.36620333945274935</v>
       </c>
@@ -555,7 +656,7 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -566,18 +667,18 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="7">
         <f>2930/8173</f>
         <v>0.35849749174109874</v>
       </c>
       <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -588,17 +689,17 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="7">
         <v>0.35580000000000001</v>
       </c>
       <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -609,17 +710,17 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="7">
         <v>0.3493</v>
       </c>
       <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -630,17 +731,278 @@
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="7">
         <v>0.3458</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="F10" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="8">
+        <v>762</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <f>A14+1</f>
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="8">
+        <v>755</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <f t="shared" ref="A16:A18" si="1">A15+1</f>
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="8">
+        <v>714</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="8">
+        <v>696</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="8">
+        <v>660</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="8">
+        <v>656</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>26</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2297</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <f>A23+1</f>
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2214</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <f t="shared" ref="A25:A27" si="2">A24+1</f>
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2086</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2075</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2075</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setting up app for heroku deployment
</commit_message>
<xml_diff>
--- a/TCT-database.xlsx
+++ b/TCT-database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waltersylvester/sei-cranberry-gobblers/project-1-the-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98335C80-2EDB-6E43-AF76-B7996E503B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1517049C-473C-9945-A290-E31BAABFBFC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6080" yWindow="1560" windowWidth="24740" windowHeight="17440" xr2:uid="{94078475-5FDC-3F47-8680-DE6E559C9F43}"/>
   </bookViews>
@@ -204,7 +204,7 @@
     <t>13th round pick in 1999</t>
   </si>
   <si>
-    <t>3-time MVP, 6-time Silver Slugger</t>
+    <t>3-time MVP and 6-time Silver Slugger</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <dimension ref="A2:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -945,7 +945,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <f t="shared" ref="A25:A27" si="2">A24+1</f>
+        <f t="shared" ref="A25:A26" si="2">A24+1</f>
         <v>3</v>
       </c>
       <c r="B25" t="s">

</xml_diff>